<commit_message>
Actually (mostly) working code. Fixes to almost everything.
</commit_message>
<xml_diff>
--- a/Test_L8.xlsx
+++ b/Test_L8.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TaguchiOA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C903A6-B040-4985-80ED-7B85FC2A538A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C96CAF5-9E1B-4F60-B60C-AF528E4C20AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{AA9E8D8C-2DB8-4F42-B53F-B0B7CBE4D9E0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="2" xr2:uid="{AA9E8D8C-2DB8-4F42-B53F-B0B7CBE4D9E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Set-up" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Heat Shock</t>
   </si>
@@ -50,29 +50,39 @@
     <t>Annealed Adapter</t>
   </si>
   <si>
-    <t>Ct Value</t>
-  </si>
-  <si>
     <t>LAA</t>
   </si>
   <si>
-    <t>Ct Value.1</t>
+    <t>LTB</t>
   </si>
   <si>
-    <t>Ct Value.2</t>
+    <t>EstimatedUnique</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -83,7 +93,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -91,12 +101,204 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,7 +616,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,89 +674,63 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20B3D2EB-78ED-4FD1-99A9-C5120BF9AA53}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>10</v>
-      </c>
-      <c r="B2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5.1856046488107603</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>11</v>
-      </c>
-      <c r="B3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5.0191349866370496</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>13</v>
-      </c>
-      <c r="B4">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4.8292193117266304</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>14</v>
-      </c>
-      <c r="B5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5.0689338678990197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>15</v>
-      </c>
-      <c r="B6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5.2208538062433796</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>16</v>
-      </c>
-      <c r="B7">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5.1770040048676798</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>17</v>
-      </c>
-      <c r="B8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5.1357813069062797</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>18</v>
-      </c>
-      <c r="B9">
-        <v>12</v>
+        <v>5.1328852563986702</v>
       </c>
     </row>
   </sheetData>
@@ -564,25 +740,500 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C49E6B53-C591-46CA-8898-EF4FC7ADBCE3}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:AF35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7:AF35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="6" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S7" s="9"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="12"/>
+      <c r="W7" s="12"/>
+      <c r="X7" s="12"/>
+      <c r="Y7" s="12"/>
+      <c r="Z7" s="12"/>
+      <c r="AA7" s="12"/>
+      <c r="AB7" s="12"/>
+      <c r="AC7" s="12"/>
+      <c r="AD7" s="12"/>
+      <c r="AE7" s="12"/>
+      <c r="AF7" s="13"/>
+    </row>
+    <row r="8" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S8" s="10"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="3"/>
+    </row>
+    <row r="9" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S9" s="4"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="5"/>
+    </row>
+    <row r="10" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S10" s="4"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="2"/>
+      <c r="AD10" s="2"/>
+      <c r="AE10" s="2"/>
+      <c r="AF10" s="5"/>
+    </row>
+    <row r="11" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S11" s="4"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="2"/>
+      <c r="AE11" s="2"/>
+      <c r="AF11" s="5"/>
+    </row>
+    <row r="12" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S12" s="4"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="2"/>
+      <c r="AE12" s="2"/>
+      <c r="AF12" s="5"/>
+    </row>
+    <row r="13" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S13" s="4"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="2"/>
+      <c r="AE13" s="2"/>
+      <c r="AF13" s="5"/>
+    </row>
+    <row r="14" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S14" s="4"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="2"/>
+      <c r="AD14" s="2"/>
+      <c r="AE14" s="2"/>
+      <c r="AF14" s="5"/>
+    </row>
+    <row r="15" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S15" s="4"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2"/>
+      <c r="AD15" s="2"/>
+      <c r="AE15" s="2"/>
+      <c r="AF15" s="5"/>
+    </row>
+    <row r="16" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S16" s="4"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="2"/>
+      <c r="AD16" s="2"/>
+      <c r="AE16" s="2"/>
+      <c r="AF16" s="5"/>
+    </row>
+    <row r="17" spans="19:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S17" s="4"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2"/>
+      <c r="Z17" s="2"/>
+      <c r="AA17" s="2"/>
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="2"/>
+      <c r="AD17" s="2"/>
+      <c r="AE17" s="2"/>
+      <c r="AF17" s="5"/>
+    </row>
+    <row r="18" spans="19:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S18" s="4"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="2"/>
+      <c r="AD18" s="2"/>
+      <c r="AE18" s="2"/>
+      <c r="AF18" s="5"/>
+    </row>
+    <row r="19" spans="19:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S19" s="4"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="2"/>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="2"/>
+      <c r="AD19" s="2"/>
+      <c r="AE19" s="2"/>
+      <c r="AF19" s="5"/>
+    </row>
+    <row r="20" spans="19:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S20" s="4"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="2"/>
+      <c r="Z20" s="2"/>
+      <c r="AA20" s="2"/>
+      <c r="AB20" s="2"/>
+      <c r="AC20" s="2"/>
+      <c r="AD20" s="2"/>
+      <c r="AE20" s="2"/>
+      <c r="AF20" s="5"/>
+    </row>
+    <row r="21" spans="19:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S21" s="4"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2"/>
+      <c r="Y21" s="2"/>
+      <c r="Z21" s="2"/>
+      <c r="AA21" s="2"/>
+      <c r="AB21" s="2"/>
+      <c r="AC21" s="2"/>
+      <c r="AD21" s="2"/>
+      <c r="AE21" s="2"/>
+      <c r="AF21" s="5"/>
+    </row>
+    <row r="22" spans="19:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S22" s="4"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="2"/>
+      <c r="Y22" s="2"/>
+      <c r="Z22" s="2"/>
+      <c r="AA22" s="2"/>
+      <c r="AB22" s="2"/>
+      <c r="AC22" s="2"/>
+      <c r="AD22" s="2"/>
+      <c r="AE22" s="2"/>
+      <c r="AF22" s="5"/>
+    </row>
+    <row r="23" spans="19:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S23" s="4"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="2"/>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2"/>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="2"/>
+      <c r="AD23" s="2"/>
+      <c r="AE23" s="2"/>
+      <c r="AF23" s="5"/>
+    </row>
+    <row r="24" spans="19:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S24" s="4"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2"/>
+      <c r="Y24" s="2"/>
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="2"/>
+      <c r="AB24" s="2"/>
+      <c r="AC24" s="2"/>
+      <c r="AD24" s="2"/>
+      <c r="AE24" s="2"/>
+      <c r="AF24" s="5"/>
+    </row>
+    <row r="25" spans="19:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S25" s="4"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="2"/>
+      <c r="Z25" s="2"/>
+      <c r="AA25" s="2"/>
+      <c r="AB25" s="2"/>
+      <c r="AC25" s="2"/>
+      <c r="AD25" s="2"/>
+      <c r="AE25" s="2"/>
+      <c r="AF25" s="5"/>
+    </row>
+    <row r="26" spans="19:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S26" s="4"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2"/>
+      <c r="Y26" s="2"/>
+      <c r="Z26" s="2"/>
+      <c r="AA26" s="2"/>
+      <c r="AB26" s="2"/>
+      <c r="AC26" s="2"/>
+      <c r="AD26" s="2"/>
+      <c r="AE26" s="2"/>
+      <c r="AF26" s="5"/>
+    </row>
+    <row r="27" spans="19:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S27" s="4"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2"/>
+      <c r="Z27" s="2"/>
+      <c r="AA27" s="2"/>
+      <c r="AB27" s="2"/>
+      <c r="AC27" s="2"/>
+      <c r="AD27" s="2"/>
+      <c r="AE27" s="2"/>
+      <c r="AF27" s="5"/>
+    </row>
+    <row r="28" spans="19:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S28" s="4"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="2"/>
+      <c r="X28" s="2"/>
+      <c r="Y28" s="2"/>
+      <c r="Z28" s="2"/>
+      <c r="AA28" s="2"/>
+      <c r="AB28" s="2"/>
+      <c r="AC28" s="2"/>
+      <c r="AD28" s="2"/>
+      <c r="AE28" s="2"/>
+      <c r="AF28" s="5"/>
+    </row>
+    <row r="29" spans="19:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S29" s="4"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+      <c r="W29" s="2"/>
+      <c r="X29" s="2"/>
+      <c r="Y29" s="2"/>
+      <c r="Z29" s="2"/>
+      <c r="AA29" s="2"/>
+      <c r="AB29" s="2"/>
+      <c r="AC29" s="2"/>
+      <c r="AD29" s="2"/>
+      <c r="AE29" s="2"/>
+      <c r="AF29" s="5"/>
+    </row>
+    <row r="30" spans="19:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S30" s="4"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+      <c r="X30" s="2"/>
+      <c r="Y30" s="2"/>
+      <c r="Z30" s="2"/>
+      <c r="AA30" s="2"/>
+      <c r="AB30" s="2"/>
+      <c r="AC30" s="2"/>
+      <c r="AD30" s="2"/>
+      <c r="AE30" s="2"/>
+      <c r="AF30" s="5"/>
+    </row>
+    <row r="31" spans="19:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S31" s="4"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2"/>
+      <c r="V31" s="2"/>
+      <c r="W31" s="2"/>
+      <c r="X31" s="2"/>
+      <c r="Y31" s="2"/>
+      <c r="Z31" s="2"/>
+      <c r="AA31" s="2"/>
+      <c r="AB31" s="2"/>
+      <c r="AC31" s="2"/>
+      <c r="AD31" s="2"/>
+      <c r="AE31" s="2"/>
+      <c r="AF31" s="5"/>
+    </row>
+    <row r="32" spans="19:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S32" s="4"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
+      <c r="V32" s="2"/>
+      <c r="W32" s="2"/>
+      <c r="X32" s="2"/>
+      <c r="Y32" s="2"/>
+      <c r="Z32" s="2"/>
+      <c r="AA32" s="2"/>
+      <c r="AB32" s="2"/>
+      <c r="AC32" s="2"/>
+      <c r="AD32" s="2"/>
+      <c r="AE32" s="2"/>
+      <c r="AF32" s="5"/>
+    </row>
+    <row r="33" spans="19:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S33" s="4"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+      <c r="W33" s="2"/>
+      <c r="X33" s="2"/>
+      <c r="Y33" s="2"/>
+      <c r="Z33" s="2"/>
+      <c r="AA33" s="2"/>
+      <c r="AB33" s="2"/>
+      <c r="AC33" s="2"/>
+      <c r="AD33" s="2"/>
+      <c r="AE33" s="2"/>
+      <c r="AF33" s="5"/>
+    </row>
+    <row r="34" spans="19:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S34" s="4"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
+      <c r="V34" s="2"/>
+      <c r="W34" s="2"/>
+      <c r="X34" s="2"/>
+      <c r="Y34" s="2"/>
+      <c r="Z34" s="2"/>
+      <c r="AA34" s="2"/>
+      <c r="AB34" s="2"/>
+      <c r="AC34" s="2"/>
+      <c r="AD34" s="2"/>
+      <c r="AE34" s="2"/>
+      <c r="AF34" s="5"/>
+    </row>
+    <row r="35" spans="19:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S35" s="6"/>
+      <c r="T35" s="7"/>
+      <c r="U35" s="7"/>
+      <c r="V35" s="7"/>
+      <c r="W35" s="7"/>
+      <c r="X35" s="7"/>
+      <c r="Y35" s="7"/>
+      <c r="Z35" s="7"/>
+      <c r="AA35" s="7"/>
+      <c r="AB35" s="7"/>
+      <c r="AC35" s="7"/>
+      <c r="AD35" s="7"/>
+      <c r="AE35" s="7"/>
+      <c r="AF35" s="8"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="S7:S8"/>
+    <mergeCell ref="T7:AF7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>